<commit_message>
Finished writing test class
</commit_message>
<xml_diff>
--- a/src/jvmTest/TestOutputFiles/LineItemWriterTests.xlsx
+++ b/src/jvmTest/TestOutputFiles/LineItemWriterTests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12088\Documents\Spring 2023\CS-481\s23-totalled\src\jvmMain\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12088\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45714D-4F29-4772-B9BE-970E3606B369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74DFC079-DD73-4CCF-9E8C-E10205D52289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>